<commit_message>
visualize and change structure
</commit_message>
<xml_diff>
--- a/results/experiments/exp2/220530_results_res-fps.xlsx
+++ b/results/experiments/exp2/220530_results_res-fps.xlsx
@@ -8,27 +8,40 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\PycharmProjects\yolov5\results\experiments\exp2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1BB39E7-9438-4A29-BBF3-E1AD052A56BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A2CF52-FDC5-4C6A-A8BD-65CDADCC52A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="899" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14305" tabRatio="899" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="220531_res_speed" sheetId="4" r:id="rId1"/>
     <sheet name="p5_models" sheetId="5" r:id="rId2"/>
-    <sheet name="220512_res_speed_old" sheetId="1" r:id="rId3"/>
-    <sheet name="p5_models_old" sheetId="2" r:id="rId4"/>
-    <sheet name="p6_models_old" sheetId="3" r:id="rId5"/>
+    <sheet name="p5_p6old_merged" sheetId="7" r:id="rId3"/>
+    <sheet name="220512_res_speed_old" sheetId="1" r:id="rId4"/>
+    <sheet name="p5_models_old" sheetId="2" r:id="rId5"/>
+    <sheet name="p6_models_old" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
-    <pivotCache cacheId="7" r:id="rId7"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="25">
   <si>
     <t>model</t>
   </si>
@@ -592,7 +605,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="20"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
@@ -601,6 +614,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -646,13 +664,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -1278,6 +1290,9 @@
       <c:pivotFmt>
         <c:idx val="10"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="12700" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1337,7 +1352,7 @@
         <c:spPr>
           <a:ln w="12700" cap="rnd">
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:schemeClr val="accent5"/>
             </a:solidFill>
             <a:prstDash val="sysDash"/>
             <a:round/>
@@ -2261,6 +2276,1946 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[220530_results_res-fps.xlsx]p5_p6old_merged!PivotTable2</c:name>
+    <c:fmtId val="2"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="2"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="3"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="4"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="5"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="6"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="7"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:tint val="86000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="8"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:tint val="72000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="9"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:tint val="58000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="10"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln w="12700" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="11"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="44000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="12"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="58000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="13"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="72000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="14"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:shade val="86000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="15"/>
+        <c:spPr>
+          <a:ln w="12700" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:tint val="44000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:prstDash val="sysDash"/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-NL"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>yolov5n</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="44000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$A$5:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>832</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>p5_p6old_merged!$B$5:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>100.08487937992599</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.727817822269103</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.597089669589799</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14.1506336869581</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5266554937871799</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3382-4AAF-9AB7-C66BC37DBC47}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$C$3:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>yolov5s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="58000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$A$5:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>832</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>p5_p6old_merged!$C$5:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>71.959699834028399</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30.556354191837599</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.5102554137734</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.2304341890096193</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5376159134009502</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3382-4AAF-9AB7-C66BC37DBC47}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$D$3:$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>yolov5m</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="72000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$A$5:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>832</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>p5_p6old_merged!$D$5:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>41.912066731213201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15.679607417666199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.4780171395026596</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0405919474061998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.7247715981241698</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-3382-4AAF-9AB7-C66BC37DBC47}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$E$3:$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>yolov5l</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:shade val="86000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$A$5:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>832</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>p5_p6old_merged!$E$5:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>23.947833965104099</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.0517208127145796</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9505020407322902</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9139090863711701</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4292487022798199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-3382-4AAF-9AB7-C66BC37DBC47}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$F$3:$F$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>yolov5n6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$A$5:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>832</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>p5_p6old_merged!$F$5:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>89.080419478133507</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.993570826720202</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.9837828343213</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.460165732513801</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6514424554009093</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000A-3382-4AAF-9AB7-C66BC37DBC47}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$G$3:$G$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>yolov5s6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="86000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$A$5:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>832</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>p5_p6old_merged!$G$5:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>63.427131905105</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.299567838387802</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.9722223115627</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.3990764139838099</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.55208660893787</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-3382-4AAF-9AB7-C66BC37DBC47}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$H$3:$H$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>yolov5m6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="72000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$A$5:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>832</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>p5_p6old_merged!$H$5:$H$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>36.2773048062135</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14.922507509837301</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.0839976620556602</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.99677243519311</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6907323240430299</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-3382-4AAF-9AB7-C66BC37DBC47}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$I$3:$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>yolov5l6</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="58000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$A$5:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>832</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>p5_p6old_merged!$I$5:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>20.637580685947899</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.8406446022365701</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.76411417849144</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8325415606437201</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4180128462414301</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-3382-4AAF-9AB7-C66BC37DBC47}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$J$3:$J$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>fps_target</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:tint val="44000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>p5_p6old_merged!$A$5:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>448</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>832</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1024</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>p5_p6old_merged!$J$5:$J$9</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-3382-4AAF-9AB7-C66BC37DBC47}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="207364592"/>
+        <c:axId val="207370832"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="207364592"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="207370832"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="207370832"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-NL"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="207364592"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-NL"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-NL"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -3417,7 +5372,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-GB"/>
@@ -4647,6 +6602,12 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="14">
+  <a:schemeClr val="accent1"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -4686,7 +6647,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6274,6 +8235,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -6322,6 +8799,49 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
+      <xdr:colOff>39333</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>160523</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>631858</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E94A49B4-397C-420B-94AF-81E2E0DA551B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
       <xdr:colOff>133349</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>14286</xdr:rowOff>
@@ -6358,7 +8878,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7617,7 +10137,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8D284D4-77B2-4DD8-9D27-2F46C8C0DDC9}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C8D284D4-77B2-4DD8-9D27-2F46C8C0DDC9}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:F9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField axis="axisCol" showAll="0">
@@ -7834,6 +10354,403 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8705770C-0D9B-44B0-80F1-96CB3B4162DD}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
+  <location ref="A3:J9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField axis="axisCol" showAll="0">
+      <items count="11">
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item h="1" m="1" x="9"/>
+        <item x="8"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="2"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="0"/>
+  </colFields>
+  <colItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of FPS" fld="8" baseField="0" baseItem="0" numFmtId="1"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="2">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="24">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="5"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="6"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="7"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="10" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="8"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="11" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="12" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="13" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="14" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="2" format="15" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="0" count="1" selected="0">
+            <x v="9"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:F8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
@@ -7915,7 +10832,7 @@
     <dataField name="Sum of FPS" fld="8" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="5">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="4" selected="0">
@@ -8002,7 +10919,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="2">
   <location ref="A3:F9" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="10">
@@ -8087,7 +11004,7 @@
     <dataField name="Sum of FPS" fld="8" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="4">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -8569,21 +11486,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC48E676-1515-406E-A8F7-CAAF90619346}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A42" sqref="A42:A46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="12.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.375" customWidth="1"/>
+    <col min="10" max="10" width="16.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8615,7 +11532,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -8647,7 +11564,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -8679,7 +11596,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -8711,7 +11628,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -8743,7 +11660,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -8775,7 +11692,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -8807,7 +11724,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -8839,7 +11756,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -8871,7 +11788,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -8903,7 +11820,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -8935,7 +11852,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -8967,7 +11884,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -8999,7 +11916,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -9031,7 +11948,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -9063,7 +11980,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -9095,7 +12012,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -9127,7 +12044,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -9159,7 +12076,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -9191,7 +12108,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -9223,7 +12140,7 @@
         <v>2850</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -9255,7 +12172,7 @@
         <v>3673</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -9287,7 +12204,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -9319,7 +12236,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -9351,7 +12268,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -9383,7 +12300,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -9415,7 +12332,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -9447,7 +12364,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -9479,7 +12396,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -9511,7 +12428,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -9543,7 +12460,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>16</v>
       </c>
@@ -9575,7 +12492,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -9607,7 +12524,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -9639,7 +12556,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -9671,7 +12588,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>17</v>
       </c>
@@ -9703,7 +12620,7 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>17</v>
       </c>
@@ -9735,7 +12652,7 @@
         <v>1969</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -9767,7 +12684,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>18</v>
       </c>
@@ -9799,7 +12716,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -9831,7 +12748,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -9863,7 +12780,7 @@
         <v>2726</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>18</v>
       </c>
@@ -9895,7 +12812,7 @@
         <v>3634</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>24</v>
       </c>
@@ -9906,7 +12823,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>24</v>
       </c>
@@ -9917,7 +12834,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>24</v>
       </c>
@@ -9928,7 +12845,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>24</v>
       </c>
@@ -9939,7 +12856,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -9959,22 +12876,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE85E93-B8E5-4A1A-90EE-9312667461DB}">
   <dimension ref="A3:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -9982,7 +12899,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -10002,7 +12919,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>256</v>
       </c>
@@ -10022,7 +12939,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>448</v>
       </c>
@@ -10042,7 +12959,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>640</v>
       </c>
@@ -10062,7 +12979,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>832</v>
       </c>
@@ -10082,7 +12999,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1024</v>
       </c>
@@ -10109,24 +13026,342 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3E8F586-377C-4273-AC75-1DFD964DFAEC}">
+  <dimension ref="A3:O20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O9" si="0">O5-64</f>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>256</v>
+      </c>
+      <c r="B5" s="5">
+        <v>100.08487937992599</v>
+      </c>
+      <c r="C5" s="5">
+        <v>71.959699834028399</v>
+      </c>
+      <c r="D5" s="5">
+        <v>41.912066731213201</v>
+      </c>
+      <c r="E5" s="5">
+        <v>23.947833965104099</v>
+      </c>
+      <c r="F5" s="5">
+        <v>89.080419478133507</v>
+      </c>
+      <c r="G5" s="5">
+        <v>63.427131905105</v>
+      </c>
+      <c r="H5" s="5">
+        <v>36.2773048062135</v>
+      </c>
+      <c r="I5" s="5">
+        <v>20.637580685947899</v>
+      </c>
+      <c r="J5" s="5">
+        <v>30</v>
+      </c>
+      <c r="O5" s="6">
+        <f t="shared" si="0"/>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>448</v>
+      </c>
+      <c r="B6" s="5">
+        <v>44.727817822269103</v>
+      </c>
+      <c r="C6" s="5">
+        <v>30.556354191837599</v>
+      </c>
+      <c r="D6" s="5">
+        <v>15.679607417666199</v>
+      </c>
+      <c r="E6" s="5">
+        <v>8.0517208127145796</v>
+      </c>
+      <c r="F6" s="5">
+        <v>46.993570826720202</v>
+      </c>
+      <c r="G6" s="5">
+        <v>29.299567838387802</v>
+      </c>
+      <c r="H6" s="5">
+        <v>14.922507509837301</v>
+      </c>
+      <c r="I6" s="5">
+        <v>7.8406446022365701</v>
+      </c>
+      <c r="J6" s="5">
+        <v>30</v>
+      </c>
+      <c r="O6" s="7">
+        <f t="shared" si="0"/>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>640</v>
+      </c>
+      <c r="B7" s="5">
+        <v>24.597089669589799</v>
+      </c>
+      <c r="C7" s="5">
+        <v>15.5102554137734</v>
+      </c>
+      <c r="D7" s="5">
+        <v>7.4780171395026596</v>
+      </c>
+      <c r="E7" s="5">
+        <v>3.9505020407322902</v>
+      </c>
+      <c r="F7" s="5">
+        <v>24.9837828343213</v>
+      </c>
+      <c r="G7" s="5">
+        <v>14.9722223115627</v>
+      </c>
+      <c r="H7" s="5">
+        <v>7.0839976620556602</v>
+      </c>
+      <c r="I7" s="5">
+        <v>3.76411417849144</v>
+      </c>
+      <c r="J7" s="5">
+        <v>30</v>
+      </c>
+      <c r="O7" s="6">
+        <f t="shared" si="0"/>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>832</v>
+      </c>
+      <c r="B8" s="5">
+        <v>14.1506336869581</v>
+      </c>
+      <c r="C8" s="5">
+        <v>8.2304341890096193</v>
+      </c>
+      <c r="D8" s="5">
+        <v>4.0405919474061998</v>
+      </c>
+      <c r="E8" s="5">
+        <v>1.9139090863711701</v>
+      </c>
+      <c r="F8" s="5">
+        <v>13.460165732513801</v>
+      </c>
+      <c r="G8" s="5">
+        <v>8.3990764139838099</v>
+      </c>
+      <c r="H8" s="5">
+        <v>3.99677243519311</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1.8325415606437201</v>
+      </c>
+      <c r="J8" s="5">
+        <v>30</v>
+      </c>
+      <c r="O8" s="7">
+        <f t="shared" si="0"/>
+        <v>448</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>1024</v>
+      </c>
+      <c r="B9" s="5">
+        <v>8.5266554937871799</v>
+      </c>
+      <c r="C9" s="5">
+        <v>5.5376159134009502</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2.7247715981241698</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1.4292487022798199</v>
+      </c>
+      <c r="F9" s="5">
+        <v>8.6514424554009093</v>
+      </c>
+      <c r="G9" s="5">
+        <v>5.55208660893787</v>
+      </c>
+      <c r="H9" s="5">
+        <v>2.6907323240430299</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1.4180128462414301</v>
+      </c>
+      <c r="J9" s="5">
+        <v>30</v>
+      </c>
+      <c r="O9" s="6">
+        <f t="shared" si="0"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <f>O11-64</f>
+        <v>576</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O11" s="8">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O12" s="3">
+        <f>O11+64</f>
+        <v>704</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O13" s="8">
+        <f t="shared" ref="O13:O20" si="1">O12+64</f>
+        <v>768</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O14" s="3">
+        <f t="shared" si="1"/>
+        <v>832</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O15" s="8">
+        <f t="shared" si="1"/>
+        <v>896</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O16" s="3">
+        <f t="shared" si="1"/>
+        <v>960</v>
+      </c>
+    </row>
+    <row r="17" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O17" s="3">
+        <f t="shared" si="1"/>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="18" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O18" s="3">
+        <f t="shared" si="1"/>
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="19" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O19" s="3">
+        <f t="shared" si="1"/>
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="20" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O20" s="3">
+        <f t="shared" si="1"/>
+        <v>1216</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.375" customWidth="1"/>
+    <col min="10" max="10" width="16.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10158,7 +13393,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -10190,7 +13425,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -10222,7 +13457,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -10254,7 +13489,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -10286,7 +13521,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -10318,7 +13553,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -10350,7 +13585,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -10382,7 +13617,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -10414,7 +13649,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -10446,7 +13681,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -10478,7 +13713,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -10510,7 +13745,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -10542,7 +13777,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -10574,7 +13809,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -10606,7 +13841,7 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -10638,7 +13873,7 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -10670,7 +13905,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -10702,7 +13937,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -10734,7 +13969,7 @@
         <v>1439</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
@@ -10766,7 +14001,7 @@
         <v>2850</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>14</v>
       </c>
@@ -10798,7 +14033,7 @@
         <v>3673</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>15</v>
       </c>
@@ -10830,7 +14065,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -10862,7 +14097,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>15</v>
       </c>
@@ -10894,7 +14129,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -10926,7 +14161,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -10958,7 +14193,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>16</v>
       </c>
@@ -10990,7 +14225,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>16</v>
       </c>
@@ -11022,7 +14257,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -11054,7 +14289,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -11086,7 +14321,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -11118,7 +14353,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>17</v>
       </c>
@@ -11150,7 +14385,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -11182,7 +14417,7 @@
         <v>1756</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>18</v>
       </c>
@@ -11214,7 +14449,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -11246,7 +14481,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>18</v>
       </c>
@@ -11278,7 +14513,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>18</v>
       </c>
@@ -11310,7 +14545,7 @@
         <v>3227</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>22</v>
       </c>
@@ -11321,7 +14556,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>22</v>
       </c>
@@ -11332,7 +14567,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -11343,7 +14578,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -11354,7 +14589,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>23</v>
       </c>
@@ -11365,7 +14600,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>23</v>
       </c>
@@ -11376,7 +14611,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>23</v>
       </c>
@@ -11387,7 +14622,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -11398,7 +14633,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>23</v>
       </c>
@@ -11415,7 +14650,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A3:F8"/>
   <sheetViews>
@@ -11423,18 +14658,18 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -11442,7 +14677,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -11462,7 +14697,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>320</v>
       </c>
@@ -11482,7 +14717,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>480</v>
       </c>
@@ -11502,7 +14737,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>640</v>
       </c>
@@ -11522,7 +14757,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>960</v>
       </c>
@@ -11548,25 +14783,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A3:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -11574,7 +14809,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -11594,7 +14829,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>256</v>
       </c>
@@ -11614,7 +14849,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>448</v>
       </c>
@@ -11634,7 +14869,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>640</v>
       </c>
@@ -11654,7 +14889,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>832</v>
       </c>
@@ -11674,7 +14909,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1024</v>
       </c>

</xml_diff>